<commit_message>
2nd edit Git Commit
</commit_message>
<xml_diff>
--- a/src/test/resources/com/qa/excel/testdata.xlsx
+++ b/src/test/resources/com/qa/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyFirstWorkspace\PageObjectModelBasics\src\test\resources\com\qa\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1B0A7D-9CF1-45EC-BCCB-07E09DA1A000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC3FC1B-76D2-42AB-865D-440E6379933F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36" yWindow="48" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{55D99A32-850A-469C-859A-F8F072C71B4E}"/>
   </bookViews>
@@ -580,7 +580,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>